<commit_message>
Corrected Refresh issue on the service thanks to Alex's guidance
</commit_message>
<xml_diff>
--- a/Meetup/GroupList.xlsx
+++ b/Meetup/GroupList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_GitHubDesktop\blogshare\Meetup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC03486-2E02-4EF2-824F-95C6A4C1EBC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385FE2A1-0307-4C67-B634-39AF1F28FD24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26496" yWindow="1320" windowWidth="20760" windowHeight="11844" xr2:uid="{FBD5F52B-69BB-4E01-BE1D-288DCE8BDE26}"/>
+    <workbookView xWindow="-23652" yWindow="2400" windowWidth="20760" windowHeight="11832" xr2:uid="{FBD5F52B-69BB-4E01-BE1D-288DCE8BDE26}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="71">
   <si>
     <t>FeedURL</t>
   </si>
@@ -612,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A01CF63-2C8A-4AFC-86FF-A4F7E98922B3}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,7 +625,7 @@
     <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -645,7 +645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -665,7 +665,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -685,7 +685,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -705,7 +705,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -725,7 +725,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -744,8 +744,11 @@
       <c r="F6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -765,7 +768,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -785,7 +788,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -805,7 +808,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -825,7 +828,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -845,7 +848,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -865,7 +868,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -885,7 +888,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -902,18 +905,18 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
         <v>18</v>
@@ -922,46 +925,34 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="F16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" t="s">
-        <v>55</v>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="J18" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J19" t="s">
         <v>2</v>
@@ -969,17 +960,9 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>70</v>
-      </c>
-      <c r="J21" t="s">
         <v>1</v>
       </c>
     </row>
@@ -990,13 +973,12 @@
     <hyperlink ref="A12" r:id="rId3" display="https://www.meetup.com/Power-BI-Community-Times" xr:uid="{67E832C8-92AF-405A-838C-E409B9DFC8E5}"/>
     <hyperlink ref="A13" r:id="rId4" display="https://www.meetup.com/Greater-Houston-Power-BI-Users-Group" xr:uid="{E47E1780-B5A5-4AD5-9E4F-A843ADE485CE}"/>
     <hyperlink ref="A14" r:id="rId5" display="https://www.meetup.com/PowerBI-Turkiye" xr:uid="{7B847705-9F4E-4F1E-841A-BB9D32F4C26A}"/>
-    <hyperlink ref="A15" r:id="rId6" display="https://www.meetup.com/Austin-Power-BI-User-Group" xr:uid="{43C10EAE-BF0F-4E0C-8493-3591275C1A09}"/>
-    <hyperlink ref="A17" r:id="rId7" display="https://www.meetup.com/New-Stars-Of-Data" xr:uid="{24A5B414-C533-4496-8C2A-2AC19AA9C595}"/>
-    <hyperlink ref="A19" r:id="rId8" display="https://www.meetup.com/powerbiusergroup" xr:uid="{446DE33F-15DA-4F3E-A557-5FC5DECB007A}"/>
-    <hyperlink ref="A20" r:id="rId9" display="https://www.meetup.com/Power-BI-Café" xr:uid="{1BA646C4-D6F8-4C4B-BFA6-8DF71E4F42F6}"/>
-    <hyperlink ref="A16" r:id="rId10" display="https://www.meetup.com/Boston_BI" xr:uid="{4219E2C4-1854-42C9-9D49-2D0E4C02447A}"/>
-    <hyperlink ref="A7" r:id="rId11" display="https://www.meetup.com/IowaPowerBI" xr:uid="{97940DDF-A8BE-4C61-85F4-AAD0212C3AFC}"/>
-    <hyperlink ref="A11" r:id="rId12" display="https://www.meetup.com/MileHiPowerBI" xr:uid="{02DADBF5-1E3F-4BCC-A5B6-009CD554F699}"/>
+    <hyperlink ref="A16" r:id="rId6" display="https://www.meetup.com/New-Stars-Of-Data" xr:uid="{24A5B414-C533-4496-8C2A-2AC19AA9C595}"/>
+    <hyperlink ref="A18" r:id="rId7" display="https://www.meetup.com/powerbiusergroup" xr:uid="{446DE33F-15DA-4F3E-A557-5FC5DECB007A}"/>
+    <hyperlink ref="A19" r:id="rId8" display="https://www.meetup.com/Power-BI-Café" xr:uid="{1BA646C4-D6F8-4C4B-BFA6-8DF71E4F42F6}"/>
+    <hyperlink ref="A15" r:id="rId9" display="https://www.meetup.com/Boston_BI" xr:uid="{4219E2C4-1854-42C9-9D49-2D0E4C02447A}"/>
+    <hyperlink ref="A7" r:id="rId10" display="https://www.meetup.com/IowaPowerBI" xr:uid="{97940DDF-A8BE-4C61-85F4-AAD0212C3AFC}"/>
+    <hyperlink ref="A11" r:id="rId11" display="https://www.meetup.com/MileHiPowerBI" xr:uid="{02DADBF5-1E3F-4BCC-A5B6-009CD554F699}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>